<commit_message>
Add sentence review column
</commit_message>
<xml_diff>
--- a/brise_plandok/review/BRISE_review.xlsx
+++ b/brise_plandok/review/BRISE_review.xlsx
@@ -13,6 +13,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="Attribute" vbProcedure="false">Label!$B$1:$B$16</definedName>
+    <definedName function="false" hidden="false" name="Attribute_Review" vbProcedure="false">Label!$X$4:$X$6</definedName>
     <definedName function="false" hidden="false" name="Ausgestaltung_und_Sonstiges" vbProcedure="false">Label!$P$4:$P$24</definedName>
     <definedName function="false" hidden="false" name="Dach" vbProcedure="false">Label!$Q$4:$Q$12</definedName>
     <definedName function="false" hidden="false" name="Einfriedungen" vbProcedure="false">Label!$L$4:$L$8</definedName>
@@ -25,7 +26,7 @@
     <definedName function="false" hidden="false" name="Meta" vbProcedure="false">Label!$T$4:$T$9</definedName>
     <definedName function="false" hidden="false" name="NoAttribute" vbProcedure="false">Label!$U$4</definedName>
     <definedName function="false" hidden="false" name="Nutzung_Widmung" vbProcedure="false">Label!$M$4:$M$10</definedName>
-    <definedName function="false" hidden="false" name="Review" vbProcedure="false">Label!$X$4:$X$6</definedName>
+    <definedName function="false" hidden="false" name="Sentence_Review" vbProcedure="false">Label!$Z$4:$Z$5</definedName>
     <definedName function="false" hidden="false" name="Stellplaetze_Garagen_Parkgebäude" vbProcedure="false">Label!$I$4:$I$15</definedName>
     <definedName function="false" hidden="false" name="Strassen_und_Gehsteige" vbProcedure="false">Label!$R$4:$R$9</definedName>
     <definedName function="false" hidden="false" name="Volumen" vbProcedure="false">Label!$F$4:$F$4</definedName>
@@ -41,11 +42,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="133">
   <si>
     <t xml:space="preserve">Sentence_ID</t>
   </si>
   <si>
+    <t xml:space="preserve">Review</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sentence</t>
   </si>
   <si>
@@ -58,9 +62,6 @@
     <t xml:space="preserve">Given by</t>
   </si>
   <si>
-    <t xml:space="preserve">Review</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ausgestaltung_und_Sonstiges</t>
   </si>
   <si>
@@ -109,6 +110,12 @@
     <t xml:space="preserve">NoAttribute</t>
   </si>
   <si>
+    <t xml:space="preserve">Attribute Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sentence Review</t>
+  </si>
+  <si>
     <t xml:space="preserve">VolumenUndUmbaubarerRaum</t>
   </si>
   <si>
@@ -157,6 +164,9 @@
     <t xml:space="preserve">OK</t>
   </si>
   <si>
+    <t xml:space="preserve">Done</t>
+  </si>
+  <si>
     <t xml:space="preserve">BauklasseVIHoeheMax</t>
   </si>
   <si>
@@ -197,6 +207,9 @@
   </si>
   <si>
     <t xml:space="preserve">ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question</t>
   </si>
   <si>
     <t xml:space="preserve">BauklasseVIHoeheMin</t>
@@ -722,73 +735,74 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BB345"/>
+  <dimension ref="A1:BC345"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="84.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="55" style="1" width="8.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="84.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="56" style="1" width="8.74"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,7 +812,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -807,11 +821,11 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>2</v>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>3</v>
@@ -819,11 +833,11 @@
       <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>2</v>
+      <c r="K1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>3</v>
@@ -831,11 +845,11 @@
       <c r="M1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>2</v>
+      <c r="O1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>3</v>
@@ -843,11 +857,11 @@
       <c r="Q1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>2</v>
+      <c r="S1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="T1" s="4" t="s">
         <v>3</v>
@@ -855,11 +869,11 @@
       <c r="U1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="4" t="s">
-        <v>2</v>
+      <c r="W1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="X1" s="4" t="s">
         <v>3</v>
@@ -867,11 +881,11 @@
       <c r="Y1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="4" t="s">
-        <v>2</v>
+      <c r="AA1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="AB1" s="4" t="s">
         <v>3</v>
@@ -879,11 +893,11 @@
       <c r="AC1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AE1" s="4" t="s">
-        <v>2</v>
+      <c r="AE1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="AF1" s="4" t="s">
         <v>3</v>
@@ -891,11 +905,11 @@
       <c r="AG1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AH1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AI1" s="4" t="s">
-        <v>2</v>
+      <c r="AI1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="AJ1" s="4" t="s">
         <v>3</v>
@@ -903,11 +917,11 @@
       <c r="AK1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AL1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AM1" s="4" t="s">
-        <v>2</v>
+      <c r="AM1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="AN1" s="4" t="s">
         <v>3</v>
@@ -915,11 +929,11 @@
       <c r="AO1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AP1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AQ1" s="4" t="s">
-        <v>2</v>
+      <c r="AQ1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="AR1" s="4" t="s">
         <v>3</v>
@@ -927,11 +941,11 @@
       <c r="AS1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AT1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AU1" s="4" t="s">
-        <v>2</v>
+      <c r="AU1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="AV1" s="4" t="s">
         <v>3</v>
@@ -939,11 +953,11 @@
       <c r="AW1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AX1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AY1" s="4" t="s">
-        <v>2</v>
+      <c r="AY1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="AZ1" s="4" t="s">
         <v>3</v>
@@ -951,27 +965,30 @@
       <c r="BA1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BB1" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="BC1" s="5" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AD5" s="7"/>
-      <c r="AH5" s="7"/>
-      <c r="AL5" s="7"/>
-      <c r="AP5" s="7"/>
-      <c r="AT5" s="7"/>
-      <c r="AX5" s="7"/>
-      <c r="BB5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AI5" s="7"/>
+      <c r="AM5" s="7"/>
+      <c r="AQ5" s="7"/>
+      <c r="AU5" s="7"/>
+      <c r="AY5" s="7"/>
+      <c r="BC5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1314,7 +1331,7 @@
     <row r="344" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="345" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="F1:F1048576 J1:J1048576 N1:N1048576 R1:R1048576 V1:V1048576 Z1:Z1048576 AD1:AD1048576 AH1:AH1048576 AL1:AL1048576 AP1:AP1048576 AT1:AT1048576 AX1:AX1048576 BB1:BB1048576">
+  <conditionalFormatting sqref="G1:G1048576 K1:K1048576 O1:O1048576 S1:S1048576 W1:W1048576 AA1:AA1048576 AE1:AE1048576 AI1:AI1048576 AM1:AM1048576 AQ1:AQ1048576 AU1:AU1048576 AY1:AY1048576 BC1:BC1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"OK"</formula>
     </cfRule>
@@ -1325,7 +1342,7 @@
       <formula>"MISSING"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 J1:J1048576 N1:N1048576 R1:R1048576 V1:V1048576 Z1:Z1048576 AD1:AD1048576 AH1:AH1048576 AL1:AL1048576 AP1:AP1048576 AT1:AT1048576 AX1:AX1048576 BB1:BB1048576">
+  <conditionalFormatting sqref="G1:G1048576 K1:K1048576 O1:O1048576 S1:S1048576 W1:W1048576 AA1:AA1048576 AE1:AE1048576 AI1:AI1048576 AM1:AM1048576 AQ1:AQ1048576 AU1:AU1048576 AY1:AY1048576 BC1:BC1048576">
     <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"OK"</formula>
     </cfRule>
@@ -1334,6 +1351,14 @@
     </cfRule>
     <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>"MISSING"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Question"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1351,13 +1376,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:X23"/>
+  <dimension ref="B1:Z23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X5" activeCellId="0" sqref="X5"/>
+      <selection pane="topLeft" activeCell="Z11" activeCellId="0" sqref="Z11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.55"/>
@@ -1379,6 +1404,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="42.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="16.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1444,7 +1470,10 @@
         <v>21</v>
       </c>
       <c r="X3" s="9" t="s">
-        <v>5</v>
+        <v>22</v>
+      </c>
+      <c r="Z3" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1452,55 +1481,58 @@
         <v>10</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="U4" s="0" t="s">
         <v>21</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="Z4" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,46 +1540,49 @@
         <v>13</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="X5" s="10" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="Z5" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,46 +1590,46 @@
         <v>16</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1602,37 +1637,37 @@
         <v>11</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1640,37 +1675,37 @@
         <v>19</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,34 +1713,34 @@
         <v>17</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="T9" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1713,25 +1748,25 @@
         <v>20</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1739,22 +1774,22 @@
         <v>21</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,13 +1797,13 @@
         <v>15</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,13 +1811,13 @@
         <v>12</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,10 +1825,10 @@
         <v>18</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,10 +1836,10 @@
         <v>9</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,42 +1847,42 @@
         <v>14</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P17" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P18" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P19" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P20" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P21" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P22" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P23" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Track given by attribute
</commit_message>
<xml_diff>
--- a/brise_plandok/review/BRISE_review.xlsx
+++ b/brise_plandok/review/BRISE_review.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="134">
   <si>
     <t xml:space="preserve">Sentence_ID</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t xml:space="preserve">Merkmal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count</t>
   </si>
   <si>
     <t xml:space="preserve">Given by</t>
@@ -735,14 +738,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BC345"/>
+  <dimension ref="A1:BP345"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -752,57 +755,57 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="84.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="36.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="9.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="9.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="1" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="36.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="9.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="9.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="9.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="9.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="41" style="1" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="2" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="36.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="9.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="9.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="1" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="35.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="9.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="2" width="8.38"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="56" style="1" width="8.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="46" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="56" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="61" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="1" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="1" width="35.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="66" style="1" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="2" width="8.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="69" style="1" width="8.74"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,53 +827,53 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="V1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W1" s="5" t="s">
         <v>1</v>
@@ -884,53 +887,53 @@
       <c r="Z1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AK1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AM1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AO1" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="AP1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AQ1" s="5" t="s">
         <v>1</v>
@@ -944,31 +947,70 @@
       <c r="AT1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AU1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="AV1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="AZ1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="BA1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BE1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="BF1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BG1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="BH1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="BI1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="BJ1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="BK1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="BL1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="BN1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="BO1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="BP1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -976,19 +1018,19 @@
     <row r="3" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="S5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="R5" s="7"/>
       <c r="W5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AE5" s="7"/>
-      <c r="AI5" s="7"/>
-      <c r="AM5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AL5" s="7"/>
       <c r="AQ5" s="7"/>
-      <c r="AU5" s="7"/>
-      <c r="AY5" s="7"/>
-      <c r="BC5" s="7"/>
+      <c r="AV5" s="7"/>
+      <c r="BA5" s="7"/>
+      <c r="BF5" s="7"/>
+      <c r="BK5" s="7"/>
+      <c r="BP5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1331,7 +1373,7 @@
     <row r="344" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="345" customFormat="false" ht="28.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1048576 K1:K1048576 O1:O1048576 S1:S1048576 W1:W1048576 AA1:AA1048576 AE1:AE1048576 AI1:AI1048576 AM1:AM1048576 AQ1:AQ1048576 AU1:AU1048576 AY1:AY1048576 BC1:BC1048576">
+  <conditionalFormatting sqref="H1:H1048576 M1:M1048576 R1:R1048576 W1:W1048576 AB1:AB1048576 AG1:AG1048576 AL1:AL1048576 AQ1:AQ1048576 AV1:AV1048576 BA1:BA1048576 BF1:BF1048576 BK1:BK1048576 BP1:BP1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"OK"</formula>
     </cfRule>
@@ -1342,7 +1384,7 @@
       <formula>"MISSING"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576 K1:K1048576 O1:O1048576 S1:S1048576 W1:W1048576 AA1:AA1048576 AE1:AE1048576 AI1:AI1048576 AM1:AM1048576 AQ1:AQ1048576 AU1:AU1048576 AY1:AY1048576 BC1:BC1048576">
+  <conditionalFormatting sqref="H1:H1048576 M1:M1048576 R1:R1048576 W1:W1048576 AB1:AB1048576 AG1:AG1048576 AL1:AL1048576 AQ1:AQ1048576 AV1:AV1048576 BA1:BA1048576 BF1:BF1048576 BK1:BK1048576 BP1:BP1048576">
     <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"OK"</formula>
     </cfRule>
@@ -1409,480 +1451,480 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="R3" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X3" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Z3" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="X5" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="T9" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P17" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P18" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P19" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P20" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P21" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P22" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P23" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>